<commit_message>
Actualizacion de corrida final
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
+++ b/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\eclipse-workspace\ProyectoInternexaLMMS2\src\test\resources\Datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\git\ProyectoInternexa1\com.internexa.dynamics\src\test\resources\Datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="14160" windowHeight="3870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="14160" windowHeight="3870" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProyectoSolucion" sheetId="4" r:id="rId1"/>
@@ -30,10 +30,13 @@
     <definedName name="Express" localSheetId="5">PORTUGUES!$A$2:$AA$2</definedName>
     <definedName name="ProyectoSolucion" localSheetId="6">ESPAÑOL!$A$23:$AC$32</definedName>
     <definedName name="ProyectoSolucion" localSheetId="5">PORTUGUES!$A$23:$AC$32</definedName>
-    <definedName name="ProyectoSolucion" localSheetId="0">ProyectoSolucion!$A$1:$AC$10</definedName>
+    <definedName name="ProyectoSolucion" localSheetId="0">ProyectoSolucion!$A$1:$AC$6</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="6">ESPAÑOL!$A$16:$AB$17</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="5">PORTUGUES!$A$16:$AB$17</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="1">ProyectoSolucion300!$A$1:$AB$2</definedName>
+    <definedName name="ProyectoSolucion300_1" localSheetId="6">ESPAÑOL!$A$16:$AB$17</definedName>
+    <definedName name="ProyectoSolucion300_1" localSheetId="5">PORTUGUES!$A$16:$AB$17</definedName>
+    <definedName name="ProyectoSolucion300_2" localSheetId="5">PORTUGUES!$A$16:$AB$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -431,11 +434,113 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="13" name="ProyectoSolucion30021" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Administrador\Documents\COLOMBIA-ProyectoINTERNEXA\DocumentosIniciales\ProyectoSolucion300.txt" tab="0" delimiter="|">
+      <textFields count="28">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="14" name="ProyectoSolucion3003" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Administrador\Documents\COLOMBIA-ProyectoINTERNEXA\DocumentosIniciales\ProyectoSolucion300.txt" tab="0" delimiter="|">
+      <textFields count="28">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="15" name="ProyectoSolucion30031" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Administrador\Documents\COLOMBIA-ProyectoINTERNEXA\DocumentosIniciales\ProyectoSolucion300.txt" tab="0" delimiter="|">
+      <textFields count="28">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="112">
   <si>
     <t>TxtUsuario</t>
   </si>
@@ -765,13 +870,19 @@
   </si>
   <si>
     <t>100000005-Amortizaciones</t>
+  </si>
+  <si>
+    <t>23/04/2018</t>
+  </si>
+  <si>
+    <t>24/04/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -797,13 +908,6 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -851,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -861,8 +965,6 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,15 +988,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,23 +1024,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1250,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,16 +1505,16 @@
         <v>74</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>26</v>
@@ -1408,7 +1522,7 @@
       <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="3">
         <v>70</v>
       </c>
       <c r="L2" s="3">
@@ -1433,7 +1547,7 @@
         <v>52</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>43</v>
@@ -1478,16 +1592,16 @@
         <v>75</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>82</v>
@@ -1495,7 +1609,7 @@
       <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="3">
         <v>70</v>
       </c>
       <c r="L3" s="3">
@@ -1520,7 +1634,7 @@
         <v>52</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T3" s="4" t="s">
         <v>43</v>
@@ -1565,16 +1679,16 @@
         <v>76</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>26</v>
@@ -1582,7 +1696,7 @@
       <c r="J4" s="4">
         <v>9</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="3">
         <v>40</v>
       </c>
       <c r="L4" s="3">
@@ -1607,7 +1721,7 @@
         <v>52</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>43</v>
@@ -1649,16 +1763,16 @@
         <v>77</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>82</v>
@@ -1666,7 +1780,7 @@
       <c r="J5" s="4">
         <v>9</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="3">
         <v>40</v>
       </c>
       <c r="L5" s="3">
@@ -1691,7 +1805,7 @@
         <v>52</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>43</v>
@@ -1733,16 +1847,16 @@
         <v>78</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>26</v>
@@ -1750,7 +1864,7 @@
       <c r="J6" s="4">
         <v>9</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="3">
         <v>37</v>
       </c>
       <c r="L6" s="3">
@@ -1775,7 +1889,7 @@
         <v>52</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T6" s="4" t="s">
         <v>43</v>
@@ -1816,19 +1930,19 @@
         <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>82</v>
@@ -1836,7 +1950,7 @@
       <c r="J7" s="4">
         <v>9</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="3">
         <v>37</v>
       </c>
       <c r="L7" s="3">
@@ -1861,7 +1975,7 @@
         <v>52</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T7" s="4" t="s">
         <v>43</v>
@@ -1882,7 +1996,7 @@
         <v>88</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="AA7" s="3">
         <v>4</v>
@@ -1890,524 +2004,7 @@
       <c r="AB7" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="4">
-        <v>9</v>
-      </c>
-      <c r="K8" s="7">
-        <v>70</v>
-      </c>
-      <c r="L8" s="3">
-        <v>120</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="4">
-        <v>9</v>
-      </c>
-      <c r="K9" s="7">
-        <v>70</v>
-      </c>
-      <c r="L9" s="3">
-        <v>120</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U9" s="4"/>
-      <c r="V9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W9" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="X9" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="4">
-        <v>9</v>
-      </c>
-      <c r="K10" s="7">
-        <v>40</v>
-      </c>
-      <c r="L10" s="3">
-        <v>120</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA10" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" s="4">
-        <v>9</v>
-      </c>
-      <c r="K11" s="7">
-        <v>40</v>
-      </c>
-      <c r="L11" s="3">
-        <v>120</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U11" s="4"/>
-      <c r="V11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA11" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="4">
-        <v>9</v>
-      </c>
-      <c r="K12" s="7">
-        <v>37</v>
-      </c>
-      <c r="L12" s="3">
-        <v>120</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA12" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="4">
-        <v>9</v>
-      </c>
-      <c r="K13" s="7">
-        <v>37</v>
-      </c>
-      <c r="L13" s="3">
-        <v>120</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="X13" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC13" s="3" t="s">
+      <c r="AC7" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2421,13 +2018,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X13</xm:sqref>
+          <xm:sqref>X2:X7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W13</xm:sqref>
+          <xm:sqref>W2:W7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2439,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,13 +2184,13 @@
         <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>26</v>
@@ -2682,13 +2279,13 @@
         <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>82</v>
@@ -2774,13 +2371,13 @@
         <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>26</v>
@@ -2866,13 +2463,13 @@
         <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>82</v>
@@ -2972,7 +2569,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,13 +2707,13 @@
         <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>56</v>
@@ -3196,13 +2793,13 @@
         <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>56</v>
@@ -3290,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,16 +3015,16 @@
         <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>56</v>
@@ -3496,16 +3093,16 @@
         <v>63</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>56</v>
@@ -3572,16 +3169,16 @@
         <v>58</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>56</v>
@@ -3650,16 +3247,16 @@
         <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>56</v>
@@ -3726,16 +3323,16 @@
         <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>56</v>
@@ -3806,16 +3403,16 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>56</v>
@@ -3910,20 +3507,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -4003,7 +3600,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -4083,7 +3680,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -4161,7 +3758,7 @@
       </c>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -4239,7 +3836,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -4315,7 +3912,7 @@
       </c>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -4393,7 +3990,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -4469,12 +4066,12 @@
       </c>
       <c r="Z8" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -4560,7 +4157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -4646,7 +4243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -4730,95 +4327,107 @@
       </c>
       <c r="AB13" s="3"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="L16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="9" t="s">
+      <c r="Q16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="R16" s="9" t="s">
+      <c r="R16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="S16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="T16" s="9" t="s">
+      <c r="T16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="U16" s="9" t="s">
+      <c r="U16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="V16" s="9" t="s">
+      <c r="V16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="W16" s="9" t="s">
+      <c r="W16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="X16" s="9" t="s">
+      <c r="X16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Y16" s="9" t="s">
+      <c r="Y16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Z16" s="9" t="s">
+      <c r="AC16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AA16" s="9" t="s">
+      <c r="AD16" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -4832,7 +4441,7 @@
         <v>66</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>84</v>
@@ -4880,7 +4489,7 @@
         <v>52</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V17" s="4" t="s">
         <v>30</v>
@@ -4891,17 +4500,29 @@
       <c r="X17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y17" s="3" t="s">
+      <c r="Y17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="AC17" s="3">
         <v>4</v>
       </c>
-      <c r="AA17" s="3" t="s">
+      <c r="AD17" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE17" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -4915,7 +4536,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>84</v>
@@ -4963,7 +4584,7 @@
         <v>52</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V18" s="4" t="s">
         <v>30</v>
@@ -4974,17 +4595,26 @@
       <c r="X18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y18" s="3" t="s">
+      <c r="Y18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="AC18" s="3">
         <v>4</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AD18" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -4998,7 +4628,7 @@
         <v>68</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>84</v>
@@ -5046,7 +4676,7 @@
         <v>52</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V19" s="4" t="s">
         <v>30</v>
@@ -5057,17 +4687,26 @@
       <c r="X19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y19" s="3" t="s">
+      <c r="Y19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Z19" s="3">
+      <c r="AC19" s="3">
         <v>4</v>
       </c>
-      <c r="AA19" s="3" t="s">
+      <c r="AD19" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -5081,7 +4720,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>84</v>
@@ -5129,7 +4768,7 @@
         <v>52</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V20" s="4" t="s">
         <v>30</v>
@@ -5140,22 +4779,34 @@
       <c r="X20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="Y20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z20" s="3">
+      <c r="AC20" s="3">
         <v>4</v>
       </c>
-      <c r="AA20" s="3" t="s">
+      <c r="AD20" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
@@ -5244,7 +4895,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -5300,7 +4951,7 @@
         <v>52</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>43</v>
@@ -5331,7 +4982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -5387,7 +5038,7 @@
         <v>52</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>43</v>
@@ -5418,7 +5069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -5474,7 +5125,7 @@
         <v>52</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T26" s="4" t="s">
         <v>43</v>
@@ -5502,7 +5153,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -5558,7 +5209,7 @@
         <v>52</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>43</v>
@@ -5586,7 +5237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -5642,7 +5293,7 @@
         <v>52</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>43</v>
@@ -5672,7 +5323,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -5728,7 +5379,7 @@
         <v>52</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T29" s="4" t="s">
         <v>43</v>
@@ -5758,7 +5409,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -5814,7 +5465,7 @@
         <v>52</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T30" s="4" t="s">
         <v>43</v>
@@ -5842,7 +5493,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
@@ -5898,7 +5549,7 @@
         <v>52</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T31" s="4" t="s">
         <v>43</v>
@@ -5926,7 +5577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
@@ -5982,7 +5633,7 @@
         <v>52</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>43</v>
@@ -6069,7 +5720,7 @@
         <v>52</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T33" s="4" t="s">
         <v>43</v>
@@ -6156,7 +5807,7 @@
         <v>52</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T34" s="4" t="s">
         <v>43</v>
@@ -6245,7 +5896,7 @@
         <v>52</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="T35" s="4" t="s">
         <v>43</v>
@@ -6288,13 +5939,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X24:X35 U3:U8 W12:W13</xm:sqref>
+          <xm:sqref>X24:X35 U3:U8 W12:W13 Z17:Z20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>W24:W35 T3:T8 V12:V13</xm:sqref>
+          <xm:sqref>W24:W35 T3:T8 V12:V13 Y17:Y20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6304,20 +5955,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -6397,7 +6048,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -6477,7 +6128,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -6555,7 +6206,7 @@
       </c>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -6633,7 +6284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -6709,7 +6360,7 @@
       </c>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -6787,7 +6438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -6863,12 +6514,12 @@
       </c>
       <c r="Z8" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -6954,7 +6605,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -7040,7 +6691,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -7124,95 +6775,107 @@
       </c>
       <c r="AB13" s="3"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="L16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="9" t="s">
+      <c r="Q16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="R16" s="9" t="s">
+      <c r="R16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="S16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="T16" s="9" t="s">
+      <c r="T16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="U16" s="9" t="s">
+      <c r="U16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="V16" s="9" t="s">
+      <c r="V16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="W16" s="9" t="s">
+      <c r="W16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="X16" s="9" t="s">
+      <c r="X16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Y16" s="9" t="s">
+      <c r="Y16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Z16" s="9" t="s">
+      <c r="AC16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AA16" s="9" t="s">
+      <c r="AD16" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -7274,7 +6937,7 @@
         <v>52</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V17" s="4" t="s">
         <v>30</v>
@@ -7285,17 +6948,29 @@
       <c r="X17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y17" s="3" t="s">
+      <c r="Y17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="AC17" s="3">
         <v>4</v>
       </c>
-      <c r="AA17" s="3" t="s">
+      <c r="AD17" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE17" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -7357,7 +7032,7 @@
         <v>52</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V18" s="4" t="s">
         <v>30</v>
@@ -7368,17 +7043,26 @@
       <c r="X18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y18" s="3" t="s">
+      <c r="Y18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="AC18" s="3">
         <v>4</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AD18" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -7440,7 +7124,7 @@
         <v>52</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V19" s="4" t="s">
         <v>30</v>
@@ -7451,17 +7135,26 @@
       <c r="X19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y19" s="3" t="s">
+      <c r="Y19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Z19" s="3">
+      <c r="AC19" s="3">
         <v>4</v>
       </c>
-      <c r="AA19" s="3" t="s">
+      <c r="AD19" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -7523,7 +7216,7 @@
         <v>52</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="V20" s="4" t="s">
         <v>30</v>
@@ -7534,22 +7227,34 @@
       <c r="X20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="Y20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z20" s="3">
+      <c r="AC20" s="3">
         <v>4</v>
       </c>
-      <c r="AA20" s="3" t="s">
+      <c r="AD20" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
@@ -7638,7 +7343,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -7725,7 +7430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -7812,7 +7517,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -7896,7 +7601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -7980,7 +7685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -8066,7 +7771,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -8152,7 +7857,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -8236,7 +7941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
@@ -8320,7 +8025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
@@ -8681,13 +8386,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>W12:W13 U3:U8 X24:X35</xm:sqref>
+          <xm:sqref>W12:W13 U3:U8 X24:X35 Z17:Z20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>V12:V13 T3:T8 W24:W35</xm:sqref>
+          <xm:sqref>V12:V13 T3:T8 W24:W35 Y17:Y20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Actualizacion de funciones de espera
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
+++ b/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="14160" windowHeight="3870" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="14160" windowHeight="3870"/>
   </bookViews>
   <sheets>
     <sheet name="ProyectoSolucion" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="Express" localSheetId="5">PORTUGUES!$A$2:$AA$2</definedName>
     <definedName name="ProyectoSolucion" localSheetId="6">ESPAÑOL!$A$23:$AC$32</definedName>
     <definedName name="ProyectoSolucion" localSheetId="5">PORTUGUES!$A$23:$AC$32</definedName>
-    <definedName name="ProyectoSolucion" localSheetId="0">ProyectoSolucion!$A$1:$AC$6</definedName>
+    <definedName name="ProyectoSolucion" localSheetId="0">ProyectoSolucion!$A$1:$AC$3</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="6">ESPAÑOL!$A$16:$AB$17</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="5">PORTUGUES!$A$16:$AB$17</definedName>
     <definedName name="ProyectoSolucion300" localSheetId="1">ProyectoSolucion300!$A$1:$AB$2</definedName>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="112">
   <si>
     <t>TxtUsuario</t>
   </si>
@@ -988,27 +988,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1024,23 +1024,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1364,9 +1364,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1589,7 +1589,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>25</v>
@@ -1610,7 +1610,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="3">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="L3" s="3">
         <v>120</v>
@@ -1639,12 +1639,14 @@
       <c r="T3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="V3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>101</v>
@@ -1653,359 +1655,13 @@
         <v>88</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="AA3" s="3">
         <v>4</v>
       </c>
       <c r="AB3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="4">
-        <v>9</v>
-      </c>
-      <c r="K4" s="3">
-        <v>40</v>
-      </c>
-      <c r="L4" s="3">
-        <v>120</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="4"/>
-      <c r="V4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5" s="4">
-        <v>9</v>
-      </c>
-      <c r="K5" s="3">
-        <v>40</v>
-      </c>
-      <c r="L5" s="3">
-        <v>120</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="4">
-        <v>9</v>
-      </c>
-      <c r="K6" s="3">
-        <v>37</v>
-      </c>
-      <c r="L6" s="3">
-        <v>120</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" s="4">
-        <v>9</v>
-      </c>
-      <c r="K7" s="3">
-        <v>37</v>
-      </c>
-      <c r="L7" s="3">
-        <v>120</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>4</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2018,13 +1674,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X7</xm:sqref>
+          <xm:sqref>X2:X3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W7</xm:sqref>
+          <xm:sqref>W2:W3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2037,7 +1693,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E5" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,7 +2225,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,7 +2543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
@@ -3509,8 +3165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5957,8 +5613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualizacion de datadriven para estabilizar
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
+++ b/src/test/resources/Datadriven/DataDrivenInternexa.xlsx
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="114">
   <si>
     <t>TxtUsuario</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t>24/04/2018</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>20%</t>
   </si>
 </sst>
 </file>
@@ -988,27 +994,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1024,23 +1030,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Express" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion300" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Expres300" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ProyectoSolucion" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1364,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1382,7 @@
     <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1522,7 +1528,7 @@
       <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="7">
         <v>70</v>
       </c>
       <c r="L2" s="3">
@@ -1589,7 +1595,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>25</v>
@@ -1598,7 +1604,7 @@
         <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>111</v>
@@ -1609,8 +1615,8 @@
       <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="3">
-        <v>37</v>
+      <c r="K3" s="7">
+        <v>70</v>
       </c>
       <c r="L3" s="3">
         <v>120</v>
@@ -1639,14 +1645,12 @@
       <c r="T3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="U3" s="4"/>
       <c r="V3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>101</v>
@@ -1655,12 +1659,101 @@
         <v>88</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="AA3" s="3">
         <v>4</v>
       </c>
       <c r="AB3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4">
+        <v>9</v>
+      </c>
+      <c r="K4" s="7">
+        <v>37</v>
+      </c>
+      <c r="L4" s="3">
+        <v>120</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1674,13 +1767,13 @@
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X3</xm:sqref>
+          <xm:sqref>X2:X4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W3</xm:sqref>
+          <xm:sqref>W2:W4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1693,7 +1786,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E2:E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,7 +2318,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2453,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>110</v>
@@ -2446,7 +2539,7 @@
         <v>65</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>110</v>
@@ -2544,7 +2637,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2764,7 @@
         <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>110</v>
@@ -2749,7 +2842,7 @@
         <v>63</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>110</v>
@@ -2825,7 +2918,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>110</v>
@@ -2903,7 +2996,7 @@
         <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>110</v>
@@ -2979,7 +3072,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>110</v>
@@ -3059,7 +3152,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>110</v>
@@ -3165,11 +3258,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" activeCellId="1" sqref="A24:XFD25 A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>